<commit_message>
#125 updated viewer libs for editable grid and slimmer config
</commit_message>
<xml_diff>
--- a/data/avro/person-10.xlsx
+++ b/data/avro/person-10.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -390,73 +390,94 @@
       <c r="C1" t="str">
         <v>name</v>
       </c>
+      <c r="D1" t="str">
+        <v>zipcode</v>
+      </c>
     </row>
     <row r="2">
+      <c r="A2">
+        <v>25</v>
+      </c>
       <c r="B2" t="str">
         <v>MALE</v>
       </c>
       <c r="C2" t="str">
-        <v>MPPsYun</v>
+        <v>r</v>
+      </c>
+      <c r="D2">
+        <v>631</v>
       </c>
     </row>
     <row r="3">
+      <c r="A3">
+        <v>255</v>
+      </c>
       <c r="B3" t="str">
         <v>FEMALE</v>
       </c>
       <c r="C3" t="str">
-        <v>UVcDVhxpyCziyBSiRasp</v>
+        <v>oYBuz</v>
+      </c>
+      <c r="D3">
+        <v>690</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4">
-        <v>167</v>
-      </c>
       <c r="B4" t="str">
-        <v>MALE</v>
+        <v>FEMALE</v>
       </c>
       <c r="C4" t="str">
-        <v>XTrq</v>
+        <v>xKMgdHyLw</v>
+      </c>
+      <c r="D4">
+        <v>304</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5">
-        <v>541</v>
-      </c>
       <c r="B5" t="str">
         <v>MALE</v>
       </c>
       <c r="C5" t="str">
-        <v>bRHCLEwdglb</v>
+        <v>MPPsYun</v>
+      </c>
+      <c r="D5">
+        <v>875</v>
       </c>
     </row>
     <row r="6">
+      <c r="A6">
+        <v>167</v>
+      </c>
       <c r="B6" t="str">
-        <v>FEMALE</v>
+        <v>MALE</v>
       </c>
       <c r="C6" t="str">
-        <v>g</v>
+        <v>XTrq</v>
+      </c>
+      <c r="D6">
+        <v>973</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7">
-        <v>255</v>
-      </c>
       <c r="B7" t="str">
         <v>FEMALE</v>
       </c>
       <c r="C7" t="str">
-        <v>oYBuz</v>
+        <v>g</v>
+      </c>
+      <c r="D7">
+        <v>351</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8">
-        <v>906</v>
-      </c>
       <c r="B8" t="str">
-        <v>MALE</v>
+        <v>FEMALE</v>
       </c>
       <c r="C8" t="str">
-        <v>r</v>
+        <v>ynx</v>
+      </c>
+      <c r="D8">
+        <v>525</v>
       </c>
     </row>
     <row r="9">
@@ -464,15 +485,24 @@
         <v>FEMALE</v>
       </c>
       <c r="C9" t="str">
-        <v>xKMgdHyLw</v>
+        <v>xPFZ</v>
+      </c>
+      <c r="D9">
+        <v>921</v>
       </c>
     </row>
     <row r="10">
+      <c r="A10">
+        <v>541</v>
+      </c>
       <c r="B10" t="str">
-        <v>FEMALE</v>
+        <v>MALE</v>
       </c>
       <c r="C10" t="str">
-        <v>xPFZ</v>
+        <v>bRHCLEwdglb</v>
+      </c>
+      <c r="D10">
+        <v>123</v>
       </c>
     </row>
     <row r="11">
@@ -480,12 +510,15 @@
         <v>FEMALE</v>
       </c>
       <c r="C11" t="str">
-        <v>ynx</v>
+        <v>UVcDVhxpyCziyBSiRasp</v>
+      </c>
+      <c r="D11">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C11"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D11"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>